<commit_message>
Changes for import page
</commit_message>
<xml_diff>
--- a/src/assets/AMS-Template.xlsx
+++ b/src/assets/AMS-Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yogeshgu\Desktop\Asset Management\git_dev\AMS\src\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yogeshgu\Desktop\Asset Management\AMS-BKP\Devlopement\AMS\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,30 +26,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t>productName</t>
-  </si>
-  <si>
-    <t>categoryName</t>
-  </si>
-  <si>
     <t>subCategoryName</t>
   </si>
   <si>
-    <t>brandName</t>
-  </si>
-  <si>
-    <t>unit</t>
-  </si>
-  <si>
-    <t>sku</t>
-  </si>
-  <si>
     <t>minimumqty</t>
   </si>
   <si>
-    <t>quantity</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -65,7 +47,25 @@
     <t>status</t>
   </si>
   <si>
-    <t>productImage</t>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Brand</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>SKU</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>img</t>
   </si>
 </sst>
 </file>
@@ -386,50 +386,50 @@
   <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="J1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="K1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="L1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="M1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
       </c>
       <c r="N1" t="s">
         <v>13</v>

</xml_diff>